<commit_message>
Fix conflicts by preferring local changes
</commit_message>
<xml_diff>
--- a/data/02_運用_rakuten.xlsx
+++ b/data/02_運用_rakuten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6ca29965d2a6599a/01_資産管理/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="307" documentId="13_ncr:1_{F23918F6-93A0-4FFC-9C54-3B208A91E086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF25A274-6445-407F-804B-879844F0B80E}"/>
+  <xr:revisionPtr revIDLastSave="331" documentId="13_ncr:1_{F23918F6-93A0-4FFC-9C54-3B208A91E086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D773F06B-6CDF-448E-83CE-8DFAD65DDF61}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="819" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6335" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6461" uniqueCount="439">
   <si>
     <t>約定日</t>
   </si>
@@ -1932,13 +1932,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>配当</t>
-    <rPh sb="0" eb="2">
-      <t>ハイトウ</t>
-    </rPh>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>ｉＦｒｅｅＥＴＦ　東証ＲＥＩＴ指数</t>
   </si>
   <si>
@@ -1979,6 +1972,28 @@
   </si>
   <si>
     <t>ファナック</t>
+  </si>
+  <si>
+    <t>RDW</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>REDWIRE CORP</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ＯＮＥＥＴＦ東証ＲＥＩＴ</t>
+  </si>
+  <si>
+    <t>東京瓦斯</t>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="18"/>
   </si>
 </sst>
 </file>
@@ -2377,7 +2392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -2568,19 +2583,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2713,7 +2715,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2831,9 +2833,6 @@
     <xf numFmtId="38" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2851,9 +2850,6 @@
     </xf>
     <xf numFmtId="38" fontId="0" fillId="33" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -2882,16 +2878,22 @@
     <xf numFmtId="40" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2915,28 +2917,19 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3210,7 +3203,9 @@
   </sheetPr>
   <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3220,25 +3215,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="58" t="s">
         <v>213</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58" t="s">
         <v>216</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56" t="s">
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58" t="s">
         <v>218</v>
       </c>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
       <c r="O1" s="64" t="s">
         <v>302</v>
       </c>
@@ -3248,42 +3243,42 @@
       <c r="S1" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="U1" s="50" t="s">
+      <c r="U1" s="48" t="s">
         <v>362</v>
       </c>
-      <c r="V1" s="50" t="s">
+      <c r="V1" s="48" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58" t="s">
+      <c r="C2" s="54"/>
+      <c r="D2" s="54" t="s">
         <v>211</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58" t="s">
+      <c r="G2" s="54"/>
+      <c r="H2" s="54" t="s">
         <v>211</v>
       </c>
-      <c r="I2" s="59" t="s">
+      <c r="I2" s="56" t="s">
         <v>214</v>
       </c>
       <c r="J2" s="61" t="s">
         <v>217</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="L2" s="58"/>
-      <c r="M2" s="59" t="s">
+      <c r="L2" s="54"/>
+      <c r="M2" s="56" t="s">
         <v>214</v>
       </c>
       <c r="N2" s="61" t="s">
@@ -3293,7 +3288,7 @@
         <v>212</v>
       </c>
       <c r="P2" s="63"/>
-      <c r="Q2" s="59" t="s">
+      <c r="Q2" s="56" t="s">
         <v>214</v>
       </c>
       <c r="R2" s="61" t="s">
@@ -3302,12 +3297,12 @@
       <c r="S2" s="60" t="s">
         <v>214</v>
       </c>
-      <c r="U2" s="51">
+      <c r="U2" s="49">
         <v>44145</v>
       </c>
-      <c r="V2" s="51">
+      <c r="V2" s="49">
         <f ca="1">TODAY()</f>
-        <v>46039</v>
+        <v>46057</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.45">
@@ -3317,38 +3312,38 @@
       <c r="C3" s="33" t="s">
         <v>207</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="68"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="32" t="s">
         <v>206</v>
       </c>
       <c r="G3" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="H3" s="58"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
       <c r="K3" s="32" t="s">
         <v>206</v>
       </c>
       <c r="L3" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
       <c r="O3" s="32" t="s">
         <v>206</v>
       </c>
       <c r="P3" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="Q3" s="59"/>
-      <c r="R3" s="59"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
       <c r="S3" s="60"/>
-      <c r="U3" s="56" t="s">
+      <c r="U3" s="58" t="s">
         <v>364</v>
       </c>
-      <c r="V3" s="56"/>
+      <c r="V3" s="58"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4" s="34" t="s">
@@ -3372,11 +3367,11 @@
       </c>
       <c r="F4" s="20">
         <f>SUM(F5:F100)</f>
-        <v>7971493</v>
+        <v>8362963</v>
       </c>
       <c r="G4" s="20">
         <f>SUM(G5:G100)</f>
-        <v>-3522579</v>
+        <v>-3705029</v>
       </c>
       <c r="H4" s="20">
         <f>SUM(H5:H100)</f>
@@ -3384,11 +3379,11 @@
       </c>
       <c r="I4" s="35">
         <f>SUM(F4:H4)</f>
-        <v>5251069</v>
+        <v>5460089</v>
       </c>
       <c r="J4" s="35">
         <f>SUM(J5:J100)</f>
-        <v>4184314.3326499998</v>
+        <v>4350871.9196499996</v>
       </c>
       <c r="K4" s="20">
         <f>SUM(K5:K100)</f>
@@ -3424,13 +3419,13 @@
       </c>
       <c r="S4" s="38">
         <f>SUM(E4,J4,N4,R4)</f>
-        <v>7039533.8711000001</v>
-      </c>
-      <c r="U4" s="57">
+        <v>7206091.4580999995</v>
+      </c>
+      <c r="U4" s="59">
         <f ca="1">(V2-U2)/365</f>
-        <v>5.1890410958904107</v>
-      </c>
-      <c r="V4" s="57"/>
+        <v>5.2383561643835614</v>
+      </c>
+      <c r="V4" s="59"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5" s="34" t="s">
@@ -3839,11 +3834,11 @@
       </c>
       <c r="F10" s="19">
         <f>SUMIFS(国内株式_特定!$N$2:$N$998,国内株式_特定!$B$2:$B$998,"&gt;=2026/1/1",国内株式_特定!$B$2:$B$998,"&lt;=2026/12/31",国内株式_特定!$N$2:$N$998,"&gt;=0")</f>
-        <v>325100</v>
+        <v>716570</v>
       </c>
       <c r="G10" s="19">
         <f>SUMIFS(国内株式_特定!$N$2:$N$998,国内株式_特定!$B$2:$B$998,"&gt;=2026/1/1",国内株式_特定!$B$2:$B$998,"&lt;=2026/12/31",国内株式_特定!$N$2:$N$998,"&lt;0")</f>
-        <v>-97280</v>
+        <v>-279730</v>
       </c>
       <c r="H10" s="19">
         <f>SUMIFS(国内株式_特定_配当!$H$2:$H$999,国内株式_特定_配当!$A$2:$A$999,"&gt;=2026/1/1",国内株式_特定_配当!$A$2:$A$999,"&lt;=2026/12/31")</f>
@@ -3851,11 +3846,11 @@
       </c>
       <c r="I10" s="35">
         <f t="shared" si="11"/>
-        <v>227820</v>
+        <v>436840</v>
       </c>
       <c r="J10" s="36">
         <f t="shared" si="1"/>
-        <v>181538.367</v>
+        <v>348095.95400000003</v>
       </c>
       <c r="K10" s="19">
         <f>SUMIFS(国内株式_信用!$P$2:$P$1000,国内株式_信用!$B$2:$B$1000,"&gt;=2026/1/1",国内株式_信用!$B$2:$B$1000,"&lt;=2026/12/31",国内株式_信用!$P$2:$P$1000,"&gt;=0")</f>
@@ -3891,25 +3886,20 @@
       </c>
       <c r="S10" s="38">
         <f>SUM(E10,J10,N10,R10)</f>
-        <v>181538.367</v>
+        <v>348095.95400000003</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="G16" s="49"/>
+      <c r="G16" s="47"/>
     </row>
     <row r="17" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G17" s="49"/>
+      <c r="G17" s="47"/>
     </row>
     <row r="18" spans="7:8" x14ac:dyDescent="0.45">
       <c r="H18" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F2:G2"/>
     <mergeCell ref="U3:V3"/>
     <mergeCell ref="U4:V4"/>
     <mergeCell ref="H2:H3"/>
@@ -3925,6 +3915,11 @@
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="R2:R3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6534,7 +6529,7 @@
       <c r="H70" s="9">
         <v>7.65</v>
       </c>
-      <c r="I70" s="48">
+      <c r="I70" s="46">
         <f t="shared" si="6"/>
         <v>0.77000000000000046</v>
       </c>
@@ -6608,7 +6603,7 @@
       <c r="H72" s="9">
         <v>7.65</v>
       </c>
-      <c r="I72" s="48">
+      <c r="I72" s="46">
         <f t="shared" ref="I72:I74" si="7">H72-J72</f>
         <v>0.77000000000000046</v>
       </c>
@@ -6645,7 +6640,7 @@
       <c r="H73" s="9">
         <v>7.65</v>
       </c>
-      <c r="I73" s="48">
+      <c r="I73" s="46">
         <f t="shared" si="7"/>
         <v>0.77000000000000046</v>
       </c>
@@ -6682,7 +6677,7 @@
       <c r="H74" s="9">
         <v>15.83</v>
       </c>
-      <c r="I74" s="48">
+      <c r="I74" s="46">
         <f t="shared" si="7"/>
         <v>4.4499999999999993</v>
       </c>
@@ -6714,53 +6709,54 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.59765625" style="2" customWidth="1"/>
     <col min="2" max="11" width="10.59765625" customWidth="1"/>
+    <col min="12" max="12" width="9.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="58" t="s">
         <v>418</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58" t="s">
         <v>417</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="70" t="s">
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="68" t="s">
         <v>219</v>
       </c>
-      <c r="L1" s="70"/>
+      <c r="L1" s="68"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="69" t="s">
+      <c r="C2" s="54"/>
+      <c r="D2" s="67" t="s">
         <v>419</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="69" t="s">
+      <c r="G2" s="54"/>
+      <c r="H2" s="67" t="s">
         <v>419</v>
       </c>
-      <c r="I2" s="59" t="s">
+      <c r="I2" s="56" t="s">
         <v>214</v>
       </c>
       <c r="J2" s="61" t="s">
@@ -6769,8 +6765,8 @@
       <c r="K2" s="60" t="s">
         <v>214</v>
       </c>
-      <c r="L2" s="71" t="s">
-        <v>420</v>
+      <c r="L2" s="69" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
@@ -6780,19 +6776,19 @@
       <c r="C3" s="33" t="s">
         <v>207</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="68"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="32" t="s">
         <v>206</v>
       </c>
       <c r="G3" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="H3" s="67"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
       <c r="K3" s="60"/>
-      <c r="L3" s="72"/>
+      <c r="L3" s="70"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="34" t="s">
@@ -6806,7 +6802,7 @@
         <f>SUM(C5:C100)</f>
         <v>0</v>
       </c>
-      <c r="D4" s="53">
+      <c r="D4" s="51">
         <f>SUM(D5:D100)</f>
         <v>243.62</v>
       </c>
@@ -6816,29 +6812,29 @@
       </c>
       <c r="F4" s="20">
         <f>SUM(F5:F100)</f>
-        <v>576818.71481333324</v>
+        <v>814317.63481333316</v>
       </c>
       <c r="G4" s="20">
         <f>SUM(G5:G100)</f>
         <v>-64355.0412</v>
       </c>
-      <c r="H4" s="53">
+      <c r="H4" s="51">
         <f>SUM(H5:H100)</f>
         <v>374.22</v>
       </c>
       <c r="I4" s="35">
         <f>SUM(F4:G4)</f>
-        <v>512463.67361333326</v>
+        <v>749962.59361333319</v>
       </c>
       <c r="J4" s="35">
         <f>SUM(J5:J100)</f>
-        <v>407350.30052214465</v>
+        <v>596601.31492414465</v>
       </c>
       <c r="K4" s="38">
         <f>SUM(E4,J4)</f>
-        <v>678440.30052214465</v>
-      </c>
-      <c r="L4" s="55">
+        <v>867691.31492414465</v>
+      </c>
+      <c r="L4" s="53">
         <f>D4+H4</f>
         <v>617.84</v>
       </c>
@@ -6887,7 +6883,7 @@
         <f t="shared" ref="K5:K10" si="2">SUM(E5,J5)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="54"/>
+      <c r="L5" s="52"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="34" t="s">
@@ -6933,7 +6929,7 @@
         <f t="shared" si="2"/>
         <v>170325.89595128468</v>
       </c>
-      <c r="L6" s="54"/>
+      <c r="L6" s="52"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="34" t="s">
@@ -7092,7 +7088,7 @@
       </c>
       <c r="F10" s="19">
         <f>SUMIFS(米国株式!$S$2:$S$1000,米国株式!$B$2:$B$1000,"&gt;=2026/1/1",米国株式!$B$2:$B$1000,"&lt;=2026/12/31",米国株式!$E$2:$E$1000,"=特定",米国株式!$S$2:$S$1000,"&gt;=0")</f>
-        <v>0</v>
+        <v>237498.91999999998</v>
       </c>
       <c r="G10" s="19">
         <f>SUMIFS(米国株式!$S$2:$S$1000,米国株式!$B$2:$B$1000,"&gt;=2026/1/1",米国株式!$B$2:$B$1000,"&lt;=2026/12/31",米国株式!$E$2:$E$1000,"=特定",米国株式!$S$2:$S$1000,"&lt;0")</f>
@@ -7104,22 +7100,22 @@
       </c>
       <c r="I10" s="35">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>237498.91999999998</v>
       </c>
       <c r="J10" s="36">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>189251.014402</v>
       </c>
       <c r="K10" s="38">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>189251.014402</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="G16" s="49"/>
+      <c r="G16" s="47"/>
     </row>
     <row r="17" spans="7:8" x14ac:dyDescent="0.45">
-      <c r="G17" s="49"/>
+      <c r="G17" s="47"/>
     </row>
     <row r="18" spans="7:8" x14ac:dyDescent="0.45">
       <c r="H18" s="26"/>
@@ -12238,13 +12234,13 @@
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:O793"/>
+  <dimension ref="A1:O812"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E777" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E798" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N793" sqref="N793"/>
+      <selection pane="bottomRight" activeCell="N808" sqref="N808"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -12258,7 +12254,7 @@
     <col min="9" max="9" width="15.09765625" customWidth="1"/>
     <col min="10" max="11" width="17.09765625" customWidth="1"/>
     <col min="12" max="12" width="11.19921875" customWidth="1"/>
-    <col min="13" max="13" width="19.19921875" style="43" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.19921875" style="42" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.69921875" style="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12299,10 +12295,10 @@
       <c r="L1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="M1" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="N1" s="44" t="s">
         <v>165</v>
       </c>
     </row>
@@ -29535,7 +29531,7 @@
       <c r="N384" s="21">
         <v>0</v>
       </c>
-      <c r="O384" s="42"/>
+      <c r="O384" s="41"/>
     </row>
     <row r="385" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A385" s="4">
@@ -45913,7 +45909,7 @@
         <v>90</v>
       </c>
       <c r="M748" s="15">
-        <f t="shared" ref="M748:M793" si="18">IF(G748="買付",H748*I748+SUM(J748:K748),H748*I748-SUM(J748:K748))</f>
+        <f t="shared" ref="M748:M812" si="18">IF(G748="買付",H748*I748+SUM(J748:K748),H748*I748-SUM(J748:K748))</f>
         <v>233370</v>
       </c>
       <c r="N748" s="19">
@@ -46879,7 +46875,7 @@
         <v>1488</v>
       </c>
       <c r="D770" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E770" s="5" t="s">
         <v>67</v>
@@ -46969,7 +46965,7 @@
         <v>6758</v>
       </c>
       <c r="D772" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E772" s="5" t="s">
         <v>67</v>
@@ -47014,7 +47010,7 @@
         <v>6330</v>
       </c>
       <c r="D773" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E773" s="5" t="s">
         <v>67</v>
@@ -47059,7 +47055,7 @@
         <v>6758</v>
       </c>
       <c r="D774" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E774" s="5" t="s">
         <v>67</v>
@@ -47149,7 +47145,7 @@
         <v>8001</v>
       </c>
       <c r="D776" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E776" s="5" t="s">
         <v>67</v>
@@ -47194,7 +47190,7 @@
         <v>1605</v>
       </c>
       <c r="D777" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E777" s="5" t="s">
         <v>67</v>
@@ -47236,10 +47232,10 @@
         <v>46030</v>
       </c>
       <c r="C778" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="D778" s="9" t="s">
         <v>426</v>
-      </c>
-      <c r="D778" s="9" t="s">
-        <v>427</v>
       </c>
       <c r="E778" s="5" t="s">
         <v>67</v>
@@ -47281,10 +47277,10 @@
         <v>46030</v>
       </c>
       <c r="C779" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="D779" s="9" t="s">
         <v>426</v>
-      </c>
-      <c r="D779" s="9" t="s">
-        <v>427</v>
       </c>
       <c r="E779" s="5" t="s">
         <v>67</v>
@@ -47326,10 +47322,10 @@
         <v>46030</v>
       </c>
       <c r="C780" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="D780" s="9" t="s">
         <v>426</v>
-      </c>
-      <c r="D780" s="9" t="s">
-        <v>427</v>
       </c>
       <c r="E780" s="5" t="s">
         <v>67</v>
@@ -47464,7 +47460,7 @@
         <v>6330</v>
       </c>
       <c r="D783" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E783" s="5" t="s">
         <v>67</v>
@@ -47600,7 +47596,7 @@
         <v>1488</v>
       </c>
       <c r="D786" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E786" s="5" t="s">
         <v>67</v>
@@ -47642,10 +47638,10 @@
         <v>46038</v>
       </c>
       <c r="C787" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="D787" s="9" t="s">
         <v>426</v>
-      </c>
-      <c r="D787" s="9" t="s">
-        <v>427</v>
       </c>
       <c r="E787" s="5" t="s">
         <v>67</v>
@@ -47690,7 +47686,7 @@
         <v>6269</v>
       </c>
       <c r="D788" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E788" s="5" t="s">
         <v>67</v>
@@ -47735,7 +47731,7 @@
         <v>6758</v>
       </c>
       <c r="D789" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E789" s="5" t="s">
         <v>67</v>
@@ -47781,7 +47777,7 @@
         <v>2768</v>
       </c>
       <c r="D790" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E790" s="5" t="s">
         <v>67</v>
@@ -47826,7 +47822,7 @@
         <v>6954</v>
       </c>
       <c r="D791" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E791" s="5" t="s">
         <v>67</v>
@@ -47885,13 +47881,13 @@
       <c r="H792" s="5">
         <v>100</v>
       </c>
-      <c r="I792" s="73">
+      <c r="I792" s="7">
         <v>1982</v>
       </c>
-      <c r="J792" s="74">
-        <v>0</v>
-      </c>
-      <c r="K792" s="74">
+      <c r="J792" s="9">
+        <v>0</v>
+      </c>
+      <c r="K792" s="9">
         <v>0</v>
       </c>
       <c r="L792" s="9" t="s">
@@ -47930,13 +47926,13 @@
       <c r="H793" s="5">
         <v>500</v>
       </c>
-      <c r="I793" s="73">
+      <c r="I793" s="7">
         <v>1982</v>
       </c>
       <c r="J793" s="9">
         <v>0</v>
       </c>
-      <c r="K793" s="74">
+      <c r="K793" s="9">
         <v>0</v>
       </c>
       <c r="L793" s="9" t="s">
@@ -47949,6 +47945,861 @@
       <c r="N793" s="19">
         <f>24300+97200</f>
         <v>121500</v>
+      </c>
+    </row>
+    <row r="794" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A794" s="4">
+        <v>46041</v>
+      </c>
+      <c r="B794" s="4">
+        <v>46043</v>
+      </c>
+      <c r="C794" s="5">
+        <v>3692</v>
+      </c>
+      <c r="D794" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="E794" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F794" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G794" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H794" s="5">
+        <v>100</v>
+      </c>
+      <c r="I794" s="9">
+        <v>9950</v>
+      </c>
+      <c r="J794" s="9">
+        <v>0</v>
+      </c>
+      <c r="K794" s="9">
+        <v>0</v>
+      </c>
+      <c r="L794" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M794" s="15">
+        <f t="shared" si="18"/>
+        <v>995000</v>
+      </c>
+      <c r="N794" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="795" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A795" s="4">
+        <v>46041</v>
+      </c>
+      <c r="B795" s="4">
+        <v>46043</v>
+      </c>
+      <c r="C795" s="5">
+        <v>3741</v>
+      </c>
+      <c r="D795" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="E795" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F795" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G795" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H795" s="5">
+        <v>100</v>
+      </c>
+      <c r="I795" s="9">
+        <v>3669.5</v>
+      </c>
+      <c r="J795" s="9">
+        <v>0</v>
+      </c>
+      <c r="K795" s="9">
+        <v>0</v>
+      </c>
+      <c r="L795" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M795" s="15">
+        <f t="shared" si="18"/>
+        <v>366950</v>
+      </c>
+      <c r="N795" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="796" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A796" s="4">
+        <v>46041</v>
+      </c>
+      <c r="B796" s="4">
+        <v>46043</v>
+      </c>
+      <c r="C796" s="5">
+        <v>8001</v>
+      </c>
+      <c r="D796" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="E796" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F796" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G796" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H796" s="5">
+        <v>100</v>
+      </c>
+      <c r="I796" s="9">
+        <v>2098.5</v>
+      </c>
+      <c r="J796" s="9">
+        <v>0</v>
+      </c>
+      <c r="K796" s="9">
+        <v>0</v>
+      </c>
+      <c r="L796" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M796" s="15">
+        <f t="shared" si="18"/>
+        <v>209850</v>
+      </c>
+      <c r="N796" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="797" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A797" s="4">
+        <v>46041</v>
+      </c>
+      <c r="B797" s="4">
+        <v>46043</v>
+      </c>
+      <c r="C797" s="5">
+        <v>8031</v>
+      </c>
+      <c r="D797" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="E797" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F797" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G797" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H797" s="5">
+        <v>100</v>
+      </c>
+      <c r="I797" s="9">
+        <v>5094</v>
+      </c>
+      <c r="J797" s="9">
+        <v>0</v>
+      </c>
+      <c r="K797" s="9">
+        <v>0</v>
+      </c>
+      <c r="L797" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M797" s="15">
+        <f t="shared" si="18"/>
+        <v>509400</v>
+      </c>
+      <c r="N797" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="798" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A798" s="4">
+        <v>46042</v>
+      </c>
+      <c r="B798" s="4">
+        <v>46044</v>
+      </c>
+      <c r="C798" s="5">
+        <v>6269</v>
+      </c>
+      <c r="D798" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="E798" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F798" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G798" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H798" s="5">
+        <v>100</v>
+      </c>
+      <c r="I798" s="9">
+        <v>13830</v>
+      </c>
+      <c r="J798" s="9">
+        <v>0</v>
+      </c>
+      <c r="K798" s="9">
+        <v>0</v>
+      </c>
+      <c r="L798" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M798" s="15">
+        <f t="shared" si="18"/>
+        <v>1383000</v>
+      </c>
+      <c r="N798" s="19">
+        <v>-150000</v>
+      </c>
+    </row>
+    <row r="799" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A799" s="4">
+        <v>46045</v>
+      </c>
+      <c r="B799" s="4">
+        <v>46049</v>
+      </c>
+      <c r="C799" s="5">
+        <v>1605</v>
+      </c>
+      <c r="D799" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="E799" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F799" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G799" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H799" s="5">
+        <v>100</v>
+      </c>
+      <c r="I799" s="9">
+        <v>3229</v>
+      </c>
+      <c r="J799" s="9">
+        <v>0</v>
+      </c>
+      <c r="K799" s="9">
+        <v>0</v>
+      </c>
+      <c r="L799" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M799" s="15">
+        <f t="shared" si="18"/>
+        <v>322900</v>
+      </c>
+      <c r="N799" s="19">
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="800" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A800" s="4">
+        <v>46048</v>
+      </c>
+      <c r="B800" s="4">
+        <v>46050</v>
+      </c>
+      <c r="C800" s="5">
+        <v>2556</v>
+      </c>
+      <c r="D800" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E800" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F800" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G800" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H800" s="5">
+        <v>50</v>
+      </c>
+      <c r="I800" s="7">
+        <v>2036.5</v>
+      </c>
+      <c r="J800" s="9">
+        <v>0</v>
+      </c>
+      <c r="K800" s="9">
+        <v>0</v>
+      </c>
+      <c r="L800" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M800" s="15">
+        <f t="shared" si="18"/>
+        <v>101825</v>
+      </c>
+      <c r="N800" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="801" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A801" s="4">
+        <v>46048</v>
+      </c>
+      <c r="B801" s="4">
+        <v>46050</v>
+      </c>
+      <c r="C801" s="5">
+        <v>6269</v>
+      </c>
+      <c r="D801" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="E801" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F801" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G801" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H801" s="5">
+        <v>100</v>
+      </c>
+      <c r="I801" s="7">
+        <v>14100</v>
+      </c>
+      <c r="J801" s="9">
+        <v>0</v>
+      </c>
+      <c r="K801" s="9">
+        <v>0</v>
+      </c>
+      <c r="L801" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M801" s="15">
+        <f t="shared" si="18"/>
+        <v>1410000</v>
+      </c>
+      <c r="N801" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="802" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A802" s="4">
+        <v>46048</v>
+      </c>
+      <c r="B802" s="4">
+        <v>46050</v>
+      </c>
+      <c r="C802" s="5">
+        <v>9531</v>
+      </c>
+      <c r="D802" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="E802" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F802" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G802" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H802" s="5">
+        <v>100</v>
+      </c>
+      <c r="I802" s="7">
+        <v>6713</v>
+      </c>
+      <c r="J802" s="9">
+        <v>0</v>
+      </c>
+      <c r="K802" s="9">
+        <v>0</v>
+      </c>
+      <c r="L802" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M802" s="15">
+        <f t="shared" si="18"/>
+        <v>671300</v>
+      </c>
+      <c r="N802" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="803" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A803" s="4">
+        <v>46049</v>
+      </c>
+      <c r="B803" s="4">
+        <v>46051</v>
+      </c>
+      <c r="C803" s="5">
+        <v>6330</v>
+      </c>
+      <c r="D803" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="E803" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F803" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G803" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H803" s="5">
+        <v>100</v>
+      </c>
+      <c r="I803" s="7">
+        <v>5880</v>
+      </c>
+      <c r="J803" s="9">
+        <v>0</v>
+      </c>
+      <c r="K803" s="9">
+        <v>0</v>
+      </c>
+      <c r="L803" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M803" s="15">
+        <f t="shared" si="18"/>
+        <v>588000</v>
+      </c>
+      <c r="N803" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="804" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A804" s="4">
+        <v>46051</v>
+      </c>
+      <c r="B804" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C804" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="D804" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="E804" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F804" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G804" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H804" s="5">
+        <v>200</v>
+      </c>
+      <c r="I804" s="7">
+        <v>1076.7</v>
+      </c>
+      <c r="J804" s="9">
+        <v>0</v>
+      </c>
+      <c r="K804" s="9">
+        <v>0</v>
+      </c>
+      <c r="L804" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M804" s="15">
+        <f t="shared" si="18"/>
+        <v>215340</v>
+      </c>
+      <c r="N804" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="805" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A805" s="4">
+        <v>46051</v>
+      </c>
+      <c r="B805" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C805" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="D805" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="E805" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F805" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G805" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H805" s="5">
+        <v>100</v>
+      </c>
+      <c r="I805" s="7">
+        <v>1076.5999999999999</v>
+      </c>
+      <c r="J805" s="9">
+        <v>0</v>
+      </c>
+      <c r="K805" s="9">
+        <v>0</v>
+      </c>
+      <c r="L805" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M805" s="15">
+        <f t="shared" si="18"/>
+        <v>107659.99999999999</v>
+      </c>
+      <c r="N805" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="806" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A806" s="4">
+        <v>46052</v>
+      </c>
+      <c r="B806" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C806" s="5">
+        <v>1540</v>
+      </c>
+      <c r="D806" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="E806" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F806" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G806" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H806" s="5">
+        <v>25</v>
+      </c>
+      <c r="I806" s="7">
+        <v>24380</v>
+      </c>
+      <c r="J806" s="9">
+        <v>0</v>
+      </c>
+      <c r="K806" s="9">
+        <v>0</v>
+      </c>
+      <c r="L806" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M806" s="15">
+        <f t="shared" si="18"/>
+        <v>609500</v>
+      </c>
+      <c r="N806" s="19">
+        <v>110750</v>
+      </c>
+    </row>
+    <row r="807" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A807" s="4">
+        <v>46055</v>
+      </c>
+      <c r="B807" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C807" s="5">
+        <v>6269</v>
+      </c>
+      <c r="D807" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="E807" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F807" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G807" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H807" s="5">
+        <v>100</v>
+      </c>
+      <c r="I807" s="71">
+        <v>15690</v>
+      </c>
+      <c r="J807" s="9">
+        <v>0</v>
+      </c>
+      <c r="K807" s="9">
+        <v>0</v>
+      </c>
+      <c r="L807" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M807" s="15">
+        <f t="shared" si="18"/>
+        <v>1569000</v>
+      </c>
+      <c r="N807" s="19">
+        <v>159000</v>
+      </c>
+    </row>
+    <row r="808" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A808" s="4">
+        <v>46055</v>
+      </c>
+      <c r="B808" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C808" s="5">
+        <v>9684</v>
+      </c>
+      <c r="D808" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="E808" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F808" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G808" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H808" s="5">
+        <v>100</v>
+      </c>
+      <c r="I808" s="71">
+        <v>2573.5</v>
+      </c>
+      <c r="J808" s="9">
+        <v>0</v>
+      </c>
+      <c r="K808" s="9">
+        <v>0</v>
+      </c>
+      <c r="L808" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M808" s="15">
+        <f t="shared" si="18"/>
+        <v>257350</v>
+      </c>
+      <c r="N808" s="19">
+        <v>-32450</v>
+      </c>
+    </row>
+    <row r="809" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A809" s="4">
+        <v>46056</v>
+      </c>
+      <c r="B809" s="4">
+        <v>46058</v>
+      </c>
+      <c r="C809" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="D809" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="E809" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F809" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G809" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H809" s="5">
+        <v>300</v>
+      </c>
+      <c r="I809" s="71">
+        <v>1077</v>
+      </c>
+      <c r="J809" s="9">
+        <v>0</v>
+      </c>
+      <c r="K809" s="9">
+        <v>0</v>
+      </c>
+      <c r="L809" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M809" s="15">
+        <f t="shared" si="18"/>
+        <v>323100</v>
+      </c>
+      <c r="N809" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="810" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A810" s="4">
+        <v>46057</v>
+      </c>
+      <c r="B810" s="4">
+        <v>46059</v>
+      </c>
+      <c r="C810" s="5">
+        <v>5802</v>
+      </c>
+      <c r="D810" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="E810" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F810" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G810" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H810" s="5">
+        <v>100</v>
+      </c>
+      <c r="I810" s="71">
+        <v>7863</v>
+      </c>
+      <c r="J810" s="9">
+        <v>0</v>
+      </c>
+      <c r="K810" s="9">
+        <v>0</v>
+      </c>
+      <c r="L810" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M810" s="15">
+        <f t="shared" si="18"/>
+        <v>786300</v>
+      </c>
+      <c r="N810" s="19">
+        <v>68420</v>
+      </c>
+    </row>
+    <row r="811" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A811" s="4">
+        <v>46057</v>
+      </c>
+      <c r="B811" s="4">
+        <v>46059</v>
+      </c>
+      <c r="C811" s="5">
+        <v>9531</v>
+      </c>
+      <c r="D811" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="E811" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F811" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G811" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H811" s="5">
+        <v>100</v>
+      </c>
+      <c r="I811" s="71">
+        <v>7197</v>
+      </c>
+      <c r="J811" s="9">
+        <v>0</v>
+      </c>
+      <c r="K811" s="9">
+        <v>0</v>
+      </c>
+      <c r="L811" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M811" s="15">
+        <f t="shared" si="18"/>
+        <v>719700</v>
+      </c>
+      <c r="N811" s="19">
+        <v>48400</v>
+      </c>
+    </row>
+    <row r="812" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A812" s="4">
+        <v>46057</v>
+      </c>
+      <c r="B812" s="4">
+        <v>46059</v>
+      </c>
+      <c r="C812" s="5">
+        <v>6330</v>
+      </c>
+      <c r="D812" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="E812" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F812" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G812" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H812" s="5">
+        <v>100</v>
+      </c>
+      <c r="I812" s="71">
+        <v>5880</v>
+      </c>
+      <c r="J812" s="9">
+        <v>0</v>
+      </c>
+      <c r="K812" s="9">
+        <v>0</v>
+      </c>
+      <c r="L812" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M812" s="15">
+        <f t="shared" si="18"/>
+        <v>588000</v>
+      </c>
+      <c r="N812" s="19">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -49391,8 +50242,8 @@
         <f t="shared" si="5"/>
         <v>5977</v>
       </c>
-      <c r="L37" s="42"/>
-      <c r="M37" s="42"/>
+      <c r="L37" s="41"/>
+      <c r="M37" s="41"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
@@ -49487,7 +50338,7 @@
       <c r="E40" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="F40" s="41">
+      <c r="F40" s="40">
         <v>37.5</v>
       </c>
       <c r="G40" s="5">
@@ -55316,7 +56167,7 @@
       <c r="Q50" s="4">
         <v>45398</v>
       </c>
-      <c r="R50" s="41">
+      <c r="R50" s="40">
         <v>5763.4</v>
       </c>
       <c r="S50" s="9">
@@ -55980,7 +56831,7 @@
       <c r="Q58" s="4">
         <v>45398</v>
       </c>
-      <c r="R58" s="41">
+      <c r="R58" s="40">
         <v>5700.3</v>
       </c>
       <c r="S58" s="9">
@@ -56063,7 +56914,7 @@
       <c r="Q59" s="4">
         <v>45404</v>
       </c>
-      <c r="R59" s="41">
+      <c r="R59" s="40">
         <v>32225</v>
       </c>
       <c r="S59" s="9">
@@ -56146,7 +56997,7 @@
       <c r="Q60" s="4">
         <v>45404</v>
       </c>
-      <c r="R60" s="41">
+      <c r="R60" s="40">
         <v>16002.5</v>
       </c>
       <c r="S60" s="9">
@@ -56229,7 +57080,7 @@
       <c r="Q61" s="4">
         <v>45400</v>
       </c>
-      <c r="R61" s="41">
+      <c r="R61" s="40">
         <v>0</v>
       </c>
       <c r="S61" s="9">
@@ -56312,7 +57163,7 @@
       <c r="Q62" s="4">
         <v>45398</v>
       </c>
-      <c r="R62" s="41">
+      <c r="R62" s="40">
         <v>0</v>
       </c>
       <c r="S62" s="9">
@@ -56395,7 +57246,7 @@
       <c r="Q63" s="4">
         <v>45400</v>
       </c>
-      <c r="R63" s="41">
+      <c r="R63" s="40">
         <v>5840.6</v>
       </c>
       <c r="S63" s="9">
@@ -56534,7 +57385,7 @@
       <c r="J65" s="5">
         <v>100</v>
       </c>
-      <c r="K65" s="47">
+      <c r="K65" s="45">
         <v>29.639700000000001</v>
       </c>
       <c r="L65" s="9">
@@ -59029,13 +59880,13 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:T56"/>
+  <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="K41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="N45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B46" sqref="B46"/>
+      <selection pane="bottomRight" activeCell="S54" sqref="S54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -59112,12 +59963,12 @@
       <c r="R1" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="S1" s="52" t="s">
+      <c r="S1" s="50" t="s">
         <v>414</v>
       </c>
-      <c r="T1" s="42">
+      <c r="T1" s="41">
         <f>SUM(S2:S100)</f>
-        <v>783553.67361333326</v>
+        <v>1021052.5936133333</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.45">
@@ -59236,7 +60087,7 @@
         <v>0</v>
       </c>
       <c r="S3" s="19">
-        <f t="shared" ref="S3:S54" si="0">IF(H3="USD",Q3*L3,R3)</f>
+        <f t="shared" ref="S3:S58" si="0">IF(H3="USD",Q3*L3,R3)</f>
         <v>150.21300000000002</v>
       </c>
     </row>
@@ -59286,7 +60137,7 @@
       <c r="O4" s="9">
         <v>919.99</v>
       </c>
-      <c r="P4" s="40" t="s">
+      <c r="P4" s="39" t="s">
         <v>177</v>
       </c>
       <c r="Q4" s="25">
@@ -62184,7 +63035,7 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A53" s="4">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B53" s="4">
         <v>46037</v>
@@ -62229,7 +63080,7 @@
         <v>868.36</v>
       </c>
       <c r="P53" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q53" s="9">
         <v>0</v>
@@ -62244,16 +63095,16 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A54" s="4">
-        <v>46032</v>
+        <v>46035</v>
       </c>
       <c r="B54" s="4">
         <v>46037</v>
       </c>
       <c r="C54" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="D54" s="9" t="s">
         <v>428</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>429</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>67</v>
@@ -62289,7 +63140,7 @@
         <v>769.38</v>
       </c>
       <c r="P54" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q54" s="9">
         <v>0</v>
@@ -62303,26 +63154,244 @@
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A55" s="46"/>
-      <c r="B55" s="46"/>
-      <c r="C55"/>
-      <c r="E55"/>
-      <c r="F55"/>
-      <c r="G55"/>
-      <c r="H55"/>
-      <c r="K55" s="39"/>
-      <c r="O55" s="39"/>
+      <c r="A55" s="4">
+        <v>46041</v>
+      </c>
+      <c r="B55" s="4">
+        <v>46043</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="I55" s="9">
+        <v>100</v>
+      </c>
+      <c r="J55" s="9">
+        <v>12.4171</v>
+      </c>
+      <c r="K55" s="7">
+        <v>1241.71</v>
+      </c>
+      <c r="L55" s="9">
+        <v>157.85</v>
+      </c>
+      <c r="M55" s="9">
+        <v>5.58</v>
+      </c>
+      <c r="N55" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O55" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="P55" s="21">
+        <v>196971</v>
+      </c>
+      <c r="Q55" s="9">
+        <v>0</v>
+      </c>
+      <c r="R55" s="9">
+        <v>0</v>
+      </c>
+      <c r="S55" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A56" s="46"/>
-      <c r="B56" s="46"/>
-      <c r="C56"/>
-      <c r="E56"/>
-      <c r="F56"/>
-      <c r="G56"/>
-      <c r="H56"/>
-      <c r="K56" s="39"/>
-      <c r="O56" s="39"/>
+      <c r="A56" s="4">
+        <v>46052</v>
+      </c>
+      <c r="B56" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="I56" s="9">
+        <v>25</v>
+      </c>
+      <c r="J56" s="9">
+        <v>100.97499999999999</v>
+      </c>
+      <c r="K56" s="7">
+        <v>2524.37</v>
+      </c>
+      <c r="L56" s="9">
+        <v>154.12</v>
+      </c>
+      <c r="M56" s="9">
+        <v>11.35</v>
+      </c>
+      <c r="N56" s="9">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="O56" s="7">
+        <v>2511.9</v>
+      </c>
+      <c r="P56" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="Q56" s="9">
+        <v>1481.75</v>
+      </c>
+      <c r="R56" s="9">
+        <v>0</v>
+      </c>
+      <c r="S56" s="19">
+        <f>IF(H56="USD",Q56*L56,R56)</f>
+        <v>228367.31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A57" s="4">
+        <v>46052</v>
+      </c>
+      <c r="B57" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="I57" s="9">
+        <v>100</v>
+      </c>
+      <c r="J57" s="9">
+        <v>13.0701</v>
+      </c>
+      <c r="K57" s="7">
+        <v>1307.01</v>
+      </c>
+      <c r="L57" s="9">
+        <v>154.12</v>
+      </c>
+      <c r="M57" s="9">
+        <v>5.88</v>
+      </c>
+      <c r="N57" s="9">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="O57" s="7">
+        <v>1300.55</v>
+      </c>
+      <c r="P57" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="Q57" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="R57" s="9">
+        <v>0</v>
+      </c>
+      <c r="S57" s="19">
+        <f t="shared" si="0"/>
+        <v>12.329600000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A58" s="4">
+        <v>46052</v>
+      </c>
+      <c r="B58" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="I58" s="9">
+        <v>20</v>
+      </c>
+      <c r="J58" s="9">
+        <v>43.421999999999997</v>
+      </c>
+      <c r="K58" s="7">
+        <v>868.44</v>
+      </c>
+      <c r="L58" s="9">
+        <v>154.12</v>
+      </c>
+      <c r="M58" s="9">
+        <v>3.9</v>
+      </c>
+      <c r="N58" s="9">
+        <v>0.39</v>
+      </c>
+      <c r="O58" s="7">
+        <v>864.15</v>
+      </c>
+      <c r="P58" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="Q58" s="9">
+        <v>59.17</v>
+      </c>
+      <c r="R58" s="9">
+        <v>0</v>
+      </c>
+      <c r="S58" s="19">
+        <f t="shared" si="0"/>
+        <v>9119.2803999999996</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:S1" xr:uid="{00000000-0001-0000-0500-000000000000}"/>

</xml_diff>